<commit_message>
Codebase before launch of Python version of Dynamic Factor Model
git-svn-id: http://mslinuxdb01.macrosynergy.local/repositories/Nowcast/trunk@194 b65b143d-dad5-48b2-bbf2-81d1f728c7de
</commit_message>
<xml_diff>
--- a/data/datasources.xlsx
+++ b/data/datasources.xlsx
@@ -1180,9 +1180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>